<commit_message>
Added dev tickets, session roles
</commit_message>
<xml_diff>
--- a/Project_Plan.xlsx
+++ b/Project_Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UF\ResumeProjects\BugTracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18478170-0B09-4CC0-B4C8-68C183E2BBE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26C73137-DC19-428B-949A-BD3D71F2C990}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{886EFED1-650A-4142-9A82-0722A0454DCF}"/>
   </bookViews>
@@ -881,7 +881,7 @@
       <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="E17" sqref="E17"/>
+      <selection pane="bottomRight" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1869,7 +1869,9 @@
       <c r="E16" s="31">
         <v>44167</v>
       </c>
-      <c r="F16" s="31"/>
+      <c r="F16" s="31">
+        <v>44168</v>
+      </c>
       <c r="G16" s="33"/>
       <c r="H16" s="33"/>
       <c r="I16" s="33"/>
@@ -1923,8 +1925,12 @@
       <c r="D17" s="31">
         <v>44165</v>
       </c>
-      <c r="E17" s="31"/>
-      <c r="F17" s="31"/>
+      <c r="E17" s="31">
+        <v>44168</v>
+      </c>
+      <c r="F17" s="31">
+        <v>44168</v>
+      </c>
       <c r="G17" s="33"/>
       <c r="H17" s="33"/>
       <c r="I17" s="33"/>

</xml_diff>

<commit_message>
Added admin user list page '
</commit_message>
<xml_diff>
--- a/Project_Plan.xlsx
+++ b/Project_Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1 UF\ResumeProjects\BugTracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DFE5CE3-4DE4-4404-80B0-6341F1379497}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD56BD14-5E6B-42CE-BFE8-50EC183719F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{886EFED1-650A-4142-9A82-0722A0454DCF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="52">
   <si>
     <t>Project Manager</t>
   </si>
@@ -187,6 +187,9 @@
   </si>
   <si>
     <t>1. view : login page setup</t>
+  </si>
+  <si>
+    <t>removed</t>
   </si>
 </sst>
 </file>
@@ -430,7 +433,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -478,7 +481,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="3" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -487,7 +489,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -538,6 +539,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -878,10 +882,10 @@
   <dimension ref="A1:AU48"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="G9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="G15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="B12" sqref="B12"/>
+      <selection pane="bottomRight" activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -933,10 +937,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:47" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="46" t="s">
         <v>19</v>
       </c>
     </row>
@@ -951,196 +955,196 @@
       <c r="D3" s="12"/>
       <c r="E3" s="12"/>
       <c r="F3" s="12"/>
-      <c r="G3" s="55" t="s">
+      <c r="G3" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="55"/>
-      <c r="I3" s="55"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="55"/>
-      <c r="L3" s="55"/>
-      <c r="M3" s="55"/>
-      <c r="N3" s="56"/>
-      <c r="O3" s="57" t="s">
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="53"/>
+      <c r="M3" s="53"/>
+      <c r="N3" s="54"/>
+      <c r="O3" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="P3" s="57"/>
-      <c r="Q3" s="57"/>
-      <c r="R3" s="57"/>
-      <c r="S3" s="57"/>
-      <c r="T3" s="57"/>
-      <c r="U3" s="57"/>
-      <c r="V3" s="57"/>
-      <c r="W3" s="57"/>
-      <c r="X3" s="57"/>
-      <c r="Y3" s="57"/>
-      <c r="Z3" s="57"/>
-      <c r="AA3" s="57"/>
-      <c r="AB3" s="57"/>
-      <c r="AC3" s="57"/>
-      <c r="AD3" s="57"/>
-      <c r="AE3" s="57"/>
-      <c r="AF3" s="57"/>
-      <c r="AG3" s="57"/>
-      <c r="AH3" s="57"/>
-      <c r="AI3" s="57"/>
-      <c r="AJ3" s="57"/>
-      <c r="AK3" s="57"/>
-      <c r="AL3" s="57"/>
-      <c r="AM3" s="57"/>
-      <c r="AN3" s="57"/>
-      <c r="AO3" s="57"/>
-      <c r="AP3" s="57"/>
-      <c r="AQ3" s="58"/>
-      <c r="AR3" s="58"/>
-      <c r="AS3" s="59"/>
-      <c r="AT3" s="57" t="s">
+      <c r="P3" s="55"/>
+      <c r="Q3" s="55"/>
+      <c r="R3" s="55"/>
+      <c r="S3" s="55"/>
+      <c r="T3" s="55"/>
+      <c r="U3" s="55"/>
+      <c r="V3" s="55"/>
+      <c r="W3" s="55"/>
+      <c r="X3" s="55"/>
+      <c r="Y3" s="55"/>
+      <c r="Z3" s="55"/>
+      <c r="AA3" s="55"/>
+      <c r="AB3" s="55"/>
+      <c r="AC3" s="55"/>
+      <c r="AD3" s="55"/>
+      <c r="AE3" s="55"/>
+      <c r="AF3" s="55"/>
+      <c r="AG3" s="55"/>
+      <c r="AH3" s="55"/>
+      <c r="AI3" s="55"/>
+      <c r="AJ3" s="55"/>
+      <c r="AK3" s="55"/>
+      <c r="AL3" s="55"/>
+      <c r="AM3" s="55"/>
+      <c r="AN3" s="55"/>
+      <c r="AO3" s="55"/>
+      <c r="AP3" s="55"/>
+      <c r="AQ3" s="56"/>
+      <c r="AR3" s="56"/>
+      <c r="AS3" s="57"/>
+      <c r="AT3" s="55" t="s">
         <v>49</v>
       </c>
-      <c r="AU3" s="57"/>
+      <c r="AU3" s="55"/>
     </row>
     <row r="4" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="A4" s="60" t="s">
+      <c r="A4" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="60" t="s">
+      <c r="C4" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60" t="s">
+      <c r="D4" s="58"/>
+      <c r="E4" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="60"/>
-      <c r="G4" s="50" t="s">
+      <c r="F4" s="58"/>
+      <c r="G4" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="51" t="s">
+      <c r="H4" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="51" t="s">
+      <c r="I4" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="J4" s="51" t="s">
+      <c r="J4" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="51" t="s">
+      <c r="K4" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="L4" s="51" t="s">
+      <c r="L4" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="M4" s="51" t="s">
+      <c r="M4" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="N4" s="51" t="s">
+      <c r="N4" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="O4" s="51" t="s">
+      <c r="O4" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="P4" s="51" t="s">
+      <c r="P4" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="Q4" s="51" t="s">
+      <c r="Q4" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="R4" s="51" t="s">
+      <c r="R4" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="S4" s="51" t="s">
+      <c r="S4" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="T4" s="51" t="s">
+      <c r="T4" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="U4" s="51" t="s">
+      <c r="U4" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="V4" s="51" t="s">
+      <c r="V4" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="W4" s="51" t="s">
+      <c r="W4" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="X4" s="51" t="s">
+      <c r="X4" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="Y4" s="51" t="s">
+      <c r="Y4" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="Z4" s="51" t="s">
+      <c r="Z4" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="AA4" s="51" t="s">
+      <c r="AA4" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="AB4" s="51" t="s">
+      <c r="AB4" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="AC4" s="51" t="s">
+      <c r="AC4" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="AD4" s="51" t="s">
+      <c r="AD4" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="AE4" s="51" t="s">
+      <c r="AE4" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="AF4" s="51" t="s">
+      <c r="AF4" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="AG4" s="51" t="s">
+      <c r="AG4" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="AH4" s="51" t="s">
+      <c r="AH4" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="AI4" s="51" t="s">
+      <c r="AI4" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="AJ4" s="51" t="s">
+      <c r="AJ4" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="AK4" s="51" t="s">
+      <c r="AK4" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="AL4" s="51" t="s">
+      <c r="AL4" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="AM4" s="51" t="s">
+      <c r="AM4" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="AN4" s="51" t="s">
+      <c r="AN4" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="AO4" s="51" t="s">
+      <c r="AO4" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="AP4" s="51" t="s">
+      <c r="AP4" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="AQ4" s="51" t="s">
+      <c r="AQ4" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="AR4" s="51" t="s">
+      <c r="AR4" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="AS4" s="52" t="s">
+      <c r="AS4" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="AT4" s="51" t="s">
+      <c r="AT4" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="AU4" s="51" t="s">
+      <c r="AU4" s="49" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="A5" s="60"/>
-      <c r="B5" s="60"/>
+      <c r="A5" s="58"/>
+      <c r="B5" s="58"/>
       <c r="C5" s="13" t="s">
         <v>11</v>
       </c>
@@ -1153,127 +1157,127 @@
       <c r="F5" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="53">
+      <c r="G5" s="51">
         <v>23</v>
       </c>
-      <c r="H5" s="53">
+      <c r="H5" s="51">
         <v>24</v>
       </c>
-      <c r="I5" s="53">
+      <c r="I5" s="51">
         <v>25</v>
       </c>
-      <c r="J5" s="53">
+      <c r="J5" s="51">
         <v>26</v>
       </c>
-      <c r="K5" s="53">
+      <c r="K5" s="51">
         <v>27</v>
       </c>
-      <c r="L5" s="53">
+      <c r="L5" s="51">
         <v>28</v>
       </c>
-      <c r="M5" s="53">
+      <c r="M5" s="51">
         <v>29</v>
       </c>
-      <c r="N5" s="53">
+      <c r="N5" s="51">
         <v>30</v>
       </c>
-      <c r="O5" s="53">
+      <c r="O5" s="51">
         <v>1</v>
       </c>
-      <c r="P5" s="53">
+      <c r="P5" s="51">
         <v>2</v>
       </c>
-      <c r="Q5" s="53">
+      <c r="Q5" s="51">
         <v>3</v>
       </c>
-      <c r="R5" s="53">
+      <c r="R5" s="51">
         <v>4</v>
       </c>
-      <c r="S5" s="53">
+      <c r="S5" s="51">
         <v>5</v>
       </c>
-      <c r="T5" s="53">
+      <c r="T5" s="51">
         <v>6</v>
       </c>
-      <c r="U5" s="53">
+      <c r="U5" s="51">
         <v>7</v>
       </c>
-      <c r="V5" s="53">
+      <c r="V5" s="51">
         <v>8</v>
       </c>
-      <c r="W5" s="53">
+      <c r="W5" s="51">
         <v>9</v>
       </c>
-      <c r="X5" s="53">
+      <c r="X5" s="51">
         <v>10</v>
       </c>
-      <c r="Y5" s="53">
+      <c r="Y5" s="51">
         <v>11</v>
       </c>
-      <c r="Z5" s="53">
+      <c r="Z5" s="51">
         <v>12</v>
       </c>
-      <c r="AA5" s="53">
+      <c r="AA5" s="51">
         <v>13</v>
       </c>
-      <c r="AB5" s="53">
+      <c r="AB5" s="51">
         <v>14</v>
       </c>
-      <c r="AC5" s="53">
+      <c r="AC5" s="51">
         <v>15</v>
       </c>
-      <c r="AD5" s="53">
+      <c r="AD5" s="51">
         <v>16</v>
       </c>
-      <c r="AE5" s="53">
+      <c r="AE5" s="51">
         <v>17</v>
       </c>
-      <c r="AF5" s="53">
+      <c r="AF5" s="51">
         <v>18</v>
       </c>
-      <c r="AG5" s="53">
+      <c r="AG5" s="51">
         <v>19</v>
       </c>
-      <c r="AH5" s="53">
+      <c r="AH5" s="51">
         <v>20</v>
       </c>
-      <c r="AI5" s="53">
+      <c r="AI5" s="51">
         <v>21</v>
       </c>
-      <c r="AJ5" s="53">
+      <c r="AJ5" s="51">
         <v>22</v>
       </c>
-      <c r="AK5" s="53">
+      <c r="AK5" s="51">
         <v>23</v>
       </c>
-      <c r="AL5" s="53">
+      <c r="AL5" s="51">
         <v>24</v>
       </c>
-      <c r="AM5" s="53">
+      <c r="AM5" s="51">
         <v>25</v>
       </c>
-      <c r="AN5" s="53">
+      <c r="AN5" s="51">
         <v>26</v>
       </c>
-      <c r="AO5" s="53">
+      <c r="AO5" s="51">
         <v>27</v>
       </c>
-      <c r="AP5" s="53">
+      <c r="AP5" s="51">
         <v>28</v>
       </c>
-      <c r="AQ5" s="53">
+      <c r="AQ5" s="51">
         <v>29</v>
       </c>
-      <c r="AR5" s="53">
+      <c r="AR5" s="51">
         <v>30</v>
       </c>
-      <c r="AS5" s="54">
+      <c r="AS5" s="52">
         <v>31</v>
       </c>
-      <c r="AT5" s="53">
+      <c r="AT5" s="51">
         <v>1</v>
       </c>
-      <c r="AU5" s="53">
+      <c r="AU5" s="51">
         <v>2</v>
       </c>
     </row>
@@ -1339,7 +1343,7 @@
       <c r="AU6" s="3"/>
     </row>
     <row r="7" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="A7" s="35" t="s">
+      <c r="A7" s="34" t="s">
         <v>31</v>
       </c>
       <c r="B7" s="25" t="s">
@@ -1364,8 +1368,8 @@
       <c r="K7" s="29"/>
       <c r="L7" s="29"/>
       <c r="M7" s="29"/>
-      <c r="N7" s="44"/>
-      <c r="O7" s="42"/>
+      <c r="N7" s="42"/>
+      <c r="O7" s="40"/>
       <c r="P7" s="29"/>
       <c r="Q7" s="29"/>
       <c r="R7" s="29"/>
@@ -1395,8 +1399,8 @@
       <c r="AP7" s="30"/>
       <c r="AQ7" s="28"/>
       <c r="AR7" s="28"/>
-      <c r="AS7" s="45"/>
-      <c r="AT7" s="41"/>
+      <c r="AS7" s="43"/>
+      <c r="AT7" s="39"/>
       <c r="AU7" s="28"/>
     </row>
     <row r="8" spans="1:47" x14ac:dyDescent="0.3">
@@ -1455,7 +1459,7 @@
       <c r="AU8" s="3"/>
     </row>
     <row r="9" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="A9" s="34" t="s">
+      <c r="A9" s="33" t="s">
         <v>24</v>
       </c>
       <c r="B9" s="25" t="s">
@@ -1480,8 +1484,8 @@
       <c r="K9" s="28"/>
       <c r="L9" s="28"/>
       <c r="M9" s="28"/>
-      <c r="N9" s="45"/>
-      <c r="O9" s="41"/>
+      <c r="N9" s="43"/>
+      <c r="O9" s="39"/>
       <c r="P9" s="28"/>
       <c r="Q9" s="28"/>
       <c r="R9" s="28"/>
@@ -1511,12 +1515,12 @@
       <c r="AP9" s="28"/>
       <c r="AQ9" s="28"/>
       <c r="AR9" s="28"/>
-      <c r="AS9" s="45"/>
-      <c r="AT9" s="41"/>
+      <c r="AS9" s="43"/>
+      <c r="AT9" s="39"/>
       <c r="AU9" s="28"/>
     </row>
     <row r="10" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="A10" s="34" t="s">
+      <c r="A10" s="33" t="s">
         <v>25</v>
       </c>
       <c r="B10" s="25" t="s">
@@ -1531,7 +1535,7 @@
       <c r="E10" s="26">
         <v>44160</v>
       </c>
-      <c r="F10" s="32">
+      <c r="F10" s="31">
         <v>44163</v>
       </c>
       <c r="G10" s="28"/>
@@ -1539,10 +1543,10 @@
       <c r="I10" s="27"/>
       <c r="J10" s="27"/>
       <c r="K10" s="27"/>
-      <c r="L10" s="33"/>
+      <c r="L10" s="32"/>
       <c r="M10" s="28"/>
-      <c r="N10" s="45"/>
-      <c r="O10" s="41"/>
+      <c r="N10" s="43"/>
+      <c r="O10" s="39"/>
       <c r="P10" s="28"/>
       <c r="Q10" s="28"/>
       <c r="R10" s="28"/>
@@ -1572,12 +1576,12 @@
       <c r="AP10" s="28"/>
       <c r="AQ10" s="28"/>
       <c r="AR10" s="28"/>
-      <c r="AS10" s="45"/>
-      <c r="AT10" s="41"/>
+      <c r="AS10" s="43"/>
+      <c r="AT10" s="39"/>
       <c r="AU10" s="28"/>
     </row>
     <row r="11" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="33" t="s">
         <v>26</v>
       </c>
       <c r="B11" s="25" t="s">
@@ -1602,8 +1606,8 @@
       <c r="K11" s="28"/>
       <c r="L11" s="28"/>
       <c r="M11" s="28"/>
-      <c r="N11" s="45"/>
-      <c r="O11" s="41"/>
+      <c r="N11" s="43"/>
+      <c r="O11" s="39"/>
       <c r="P11" s="28"/>
       <c r="Q11" s="28"/>
       <c r="R11" s="28"/>
@@ -1633,12 +1637,12 @@
       <c r="AP11" s="28"/>
       <c r="AQ11" s="28"/>
       <c r="AR11" s="28"/>
-      <c r="AS11" s="45"/>
-      <c r="AT11" s="41"/>
+      <c r="AS11" s="43"/>
+      <c r="AT11" s="39"/>
       <c r="AU11" s="28"/>
     </row>
     <row r="12" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="A12" s="34" t="s">
+      <c r="A12" s="33" t="s">
         <v>30</v>
       </c>
       <c r="B12" s="25" t="s">
@@ -1663,8 +1667,8 @@
       <c r="K12" s="28"/>
       <c r="L12" s="28"/>
       <c r="M12" s="28"/>
-      <c r="N12" s="45"/>
-      <c r="O12" s="41"/>
+      <c r="N12" s="43"/>
+      <c r="O12" s="39"/>
       <c r="P12" s="28"/>
       <c r="Q12" s="28"/>
       <c r="R12" s="28"/>
@@ -1694,8 +1698,8 @@
       <c r="AP12" s="28"/>
       <c r="AQ12" s="28"/>
       <c r="AR12" s="28"/>
-      <c r="AS12" s="45"/>
-      <c r="AT12" s="41"/>
+      <c r="AS12" s="43"/>
+      <c r="AT12" s="39"/>
       <c r="AU12" s="28"/>
     </row>
     <row r="13" spans="1:47" x14ac:dyDescent="0.3">
@@ -1758,63 +1762,65 @@
       <c r="AU13" s="3"/>
     </row>
     <row r="14" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="A14" s="49" t="s">
+      <c r="A14" s="47" t="s">
         <v>50</v>
       </c>
-      <c r="B14" s="36"/>
-      <c r="C14" s="37">
+      <c r="B14" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="35">
         <v>44162</v>
       </c>
-      <c r="D14" s="37">
+      <c r="D14" s="35">
         <v>44162</v>
       </c>
-      <c r="E14" s="37">
+      <c r="E14" s="35">
         <v>44162</v>
       </c>
-      <c r="F14" s="37">
+      <c r="F14" s="35">
         <v>44162</v>
       </c>
-      <c r="G14" s="38"/>
-      <c r="H14" s="38"/>
-      <c r="I14" s="38"/>
-      <c r="J14" s="38"/>
-      <c r="K14" s="39"/>
-      <c r="L14" s="38"/>
-      <c r="M14" s="38"/>
-      <c r="N14" s="40"/>
-      <c r="O14" s="38"/>
-      <c r="P14" s="38"/>
-      <c r="Q14" s="38"/>
-      <c r="R14" s="38"/>
-      <c r="S14" s="38"/>
-      <c r="T14" s="38"/>
-      <c r="U14" s="38"/>
-      <c r="V14" s="38"/>
-      <c r="W14" s="38"/>
-      <c r="X14" s="38"/>
-      <c r="Y14" s="38"/>
-      <c r="Z14" s="38"/>
-      <c r="AA14" s="38"/>
-      <c r="AB14" s="38"/>
-      <c r="AC14" s="38"/>
-      <c r="AD14" s="38"/>
-      <c r="AE14" s="38"/>
-      <c r="AF14" s="38"/>
-      <c r="AG14" s="38"/>
-      <c r="AH14" s="38"/>
-      <c r="AI14" s="38"/>
-      <c r="AJ14" s="38"/>
-      <c r="AK14" s="38"/>
-      <c r="AL14" s="38"/>
-      <c r="AM14" s="38"/>
-      <c r="AN14" s="38"/>
-      <c r="AO14" s="38"/>
-      <c r="AP14" s="38"/>
-      <c r="AQ14" s="38"/>
-      <c r="AR14" s="38"/>
-      <c r="AS14" s="40"/>
-      <c r="AT14" s="38"/>
-      <c r="AU14" s="41"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="36"/>
+      <c r="I14" s="36"/>
+      <c r="J14" s="36"/>
+      <c r="K14" s="37"/>
+      <c r="L14" s="36"/>
+      <c r="M14" s="36"/>
+      <c r="N14" s="38"/>
+      <c r="O14" s="36"/>
+      <c r="P14" s="36"/>
+      <c r="Q14" s="36"/>
+      <c r="R14" s="36"/>
+      <c r="S14" s="36"/>
+      <c r="T14" s="36"/>
+      <c r="U14" s="36"/>
+      <c r="V14" s="36"/>
+      <c r="W14" s="36"/>
+      <c r="X14" s="36"/>
+      <c r="Y14" s="36"/>
+      <c r="Z14" s="36"/>
+      <c r="AA14" s="36"/>
+      <c r="AB14" s="36"/>
+      <c r="AC14" s="36"/>
+      <c r="AD14" s="36"/>
+      <c r="AE14" s="36"/>
+      <c r="AF14" s="36"/>
+      <c r="AG14" s="36"/>
+      <c r="AH14" s="36"/>
+      <c r="AI14" s="36"/>
+      <c r="AJ14" s="36"/>
+      <c r="AK14" s="36"/>
+      <c r="AL14" s="36"/>
+      <c r="AM14" s="36"/>
+      <c r="AN14" s="36"/>
+      <c r="AO14" s="36"/>
+      <c r="AP14" s="36"/>
+      <c r="AQ14" s="36"/>
+      <c r="AR14" s="36"/>
+      <c r="AS14" s="38"/>
+      <c r="AT14" s="36"/>
+      <c r="AU14" s="39"/>
     </row>
     <row r="15" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
@@ -1872,7 +1878,7 @@
       <c r="AU15" s="3"/>
     </row>
     <row r="16" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="A16" s="34" t="s">
+      <c r="A16" s="33" t="s">
         <v>24</v>
       </c>
       <c r="B16" s="25" t="s">
@@ -1897,8 +1903,8 @@
       <c r="K16" s="28"/>
       <c r="L16" s="28"/>
       <c r="M16" s="28"/>
-      <c r="N16" s="46"/>
-      <c r="O16" s="41"/>
+      <c r="N16" s="44"/>
+      <c r="O16" s="39"/>
       <c r="P16" s="28"/>
       <c r="Q16" s="28"/>
       <c r="R16" s="28"/>
@@ -1928,12 +1934,12 @@
       <c r="AP16" s="28"/>
       <c r="AQ16" s="28"/>
       <c r="AR16" s="28"/>
-      <c r="AS16" s="45"/>
-      <c r="AT16" s="41"/>
+      <c r="AS16" s="43"/>
+      <c r="AT16" s="39"/>
       <c r="AU16" s="28"/>
     </row>
     <row r="17" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="A17" s="34" t="s">
+      <c r="A17" s="33" t="s">
         <v>25</v>
       </c>
       <c r="B17" s="25" t="s">
@@ -1958,8 +1964,8 @@
       <c r="K17" s="28"/>
       <c r="L17" s="28"/>
       <c r="M17" s="28"/>
-      <c r="N17" s="46"/>
-      <c r="O17" s="41"/>
+      <c r="N17" s="44"/>
+      <c r="O17" s="39"/>
       <c r="P17" s="28"/>
       <c r="Q17" s="28"/>
       <c r="R17" s="28"/>
@@ -1989,12 +1995,12 @@
       <c r="AP17" s="28"/>
       <c r="AQ17" s="28"/>
       <c r="AR17" s="28"/>
-      <c r="AS17" s="45"/>
-      <c r="AT17" s="41"/>
+      <c r="AS17" s="43"/>
+      <c r="AT17" s="39"/>
       <c r="AU17" s="28"/>
     </row>
     <row r="18" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="A18" s="34" t="s">
+      <c r="A18" s="33" t="s">
         <v>26</v>
       </c>
       <c r="B18" s="25" t="s">
@@ -2019,11 +2025,11 @@
       <c r="K18" s="28"/>
       <c r="L18" s="28"/>
       <c r="M18" s="28"/>
-      <c r="N18" s="45"/>
-      <c r="O18" s="43"/>
+      <c r="N18" s="43"/>
+      <c r="O18" s="41"/>
       <c r="P18" s="27"/>
       <c r="Q18" s="27"/>
-      <c r="R18" s="33"/>
+      <c r="R18" s="32"/>
       <c r="S18" s="28"/>
       <c r="T18" s="28"/>
       <c r="U18" s="28"/>
@@ -2050,12 +2056,12 @@
       <c r="AP18" s="28"/>
       <c r="AQ18" s="28"/>
       <c r="AR18" s="28"/>
-      <c r="AS18" s="45"/>
-      <c r="AT18" s="41"/>
+      <c r="AS18" s="43"/>
+      <c r="AT18" s="39"/>
       <c r="AU18" s="28"/>
     </row>
     <row r="19" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="A19" s="34" t="s">
+      <c r="A19" s="33" t="s">
         <v>27</v>
       </c>
       <c r="B19" s="25" t="s">
@@ -2080,13 +2086,13 @@
       <c r="K19" s="28"/>
       <c r="L19" s="28"/>
       <c r="M19" s="28"/>
-      <c r="N19" s="45"/>
-      <c r="O19" s="41"/>
+      <c r="N19" s="43"/>
+      <c r="O19" s="39"/>
       <c r="P19" s="28"/>
       <c r="Q19" s="28"/>
       <c r="R19" s="27"/>
       <c r="S19" s="27"/>
-      <c r="T19" s="33"/>
+      <c r="T19" s="32"/>
       <c r="U19" s="28"/>
       <c r="V19" s="28"/>
       <c r="W19" s="28"/>
@@ -2111,12 +2117,12 @@
       <c r="AP19" s="28"/>
       <c r="AQ19" s="28"/>
       <c r="AR19" s="28"/>
-      <c r="AS19" s="45"/>
-      <c r="AT19" s="41"/>
+      <c r="AS19" s="43"/>
+      <c r="AT19" s="39"/>
       <c r="AU19" s="28"/>
     </row>
     <row r="20" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="A20" s="34" t="s">
+      <c r="A20" s="33" t="s">
         <v>28</v>
       </c>
       <c r="B20" s="25" t="s">
@@ -2141,8 +2147,8 @@
       <c r="K20" s="28"/>
       <c r="L20" s="28"/>
       <c r="M20" s="28"/>
-      <c r="N20" s="45"/>
-      <c r="O20" s="41"/>
+      <c r="N20" s="43"/>
+      <c r="O20" s="39"/>
       <c r="P20" s="28"/>
       <c r="Q20" s="28"/>
       <c r="R20" s="28"/>
@@ -2172,12 +2178,12 @@
       <c r="AP20" s="28"/>
       <c r="AQ20" s="28"/>
       <c r="AR20" s="28"/>
-      <c r="AS20" s="45"/>
-      <c r="AT20" s="41"/>
+      <c r="AS20" s="43"/>
+      <c r="AT20" s="39"/>
       <c r="AU20" s="28"/>
     </row>
     <row r="21" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="A21" s="34" t="s">
+      <c r="A21" s="33" t="s">
         <v>29</v>
       </c>
       <c r="B21" s="25" t="s">
@@ -2202,8 +2208,8 @@
       <c r="K21" s="28"/>
       <c r="L21" s="28"/>
       <c r="M21" s="28"/>
-      <c r="N21" s="45"/>
-      <c r="O21" s="41"/>
+      <c r="N21" s="43"/>
+      <c r="O21" s="39"/>
       <c r="P21" s="28"/>
       <c r="Q21" s="28"/>
       <c r="R21" s="28"/>
@@ -2233,8 +2239,8 @@
       <c r="AP21" s="28"/>
       <c r="AQ21" s="28"/>
       <c r="AR21" s="28"/>
-      <c r="AS21" s="45"/>
-      <c r="AT21" s="41"/>
+      <c r="AS21" s="43"/>
+      <c r="AT21" s="39"/>
       <c r="AU21" s="28"/>
     </row>
     <row r="22" spans="1:47" x14ac:dyDescent="0.3">
@@ -2293,10 +2299,12 @@
       <c r="AU22" s="3"/>
     </row>
     <row r="23" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="A23" s="34" t="s">
+      <c r="A23" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="B23" s="31"/>
+      <c r="B23" s="59" t="s">
+        <v>51</v>
+      </c>
       <c r="C23" s="26">
         <v>44183</v>
       </c>
@@ -2312,8 +2320,8 @@
       <c r="K23" s="28"/>
       <c r="L23" s="28"/>
       <c r="M23" s="28"/>
-      <c r="N23" s="45"/>
-      <c r="O23" s="41"/>
+      <c r="N23" s="43"/>
+      <c r="O23" s="39"/>
       <c r="P23" s="28"/>
       <c r="Q23" s="28"/>
       <c r="R23" s="28"/>
@@ -2343,15 +2351,15 @@
       <c r="AP23" s="28"/>
       <c r="AQ23" s="28"/>
       <c r="AR23" s="28"/>
-      <c r="AS23" s="45"/>
-      <c r="AT23" s="41"/>
+      <c r="AS23" s="43"/>
+      <c r="AT23" s="39"/>
       <c r="AU23" s="28"/>
     </row>
     <row r="24" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="A24" s="34" t="s">
+      <c r="A24" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="31"/>
+      <c r="B24" s="59"/>
       <c r="C24" s="26">
         <v>44183</v>
       </c>
@@ -2367,8 +2375,8 @@
       <c r="K24" s="28"/>
       <c r="L24" s="28"/>
       <c r="M24" s="28"/>
-      <c r="N24" s="45"/>
-      <c r="O24" s="41"/>
+      <c r="N24" s="43"/>
+      <c r="O24" s="39"/>
       <c r="P24" s="28"/>
       <c r="Q24" s="28"/>
       <c r="R24" s="28"/>
@@ -2398,15 +2406,15 @@
       <c r="AP24" s="28"/>
       <c r="AQ24" s="28"/>
       <c r="AR24" s="28"/>
-      <c r="AS24" s="45"/>
-      <c r="AT24" s="41"/>
+      <c r="AS24" s="43"/>
+      <c r="AT24" s="39"/>
       <c r="AU24" s="28"/>
     </row>
     <row r="25" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="A25" s="34" t="s">
+      <c r="A25" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="B25" s="31"/>
+      <c r="B25" s="59"/>
       <c r="C25" s="26">
         <v>44184</v>
       </c>
@@ -2422,8 +2430,8 @@
       <c r="K25" s="28"/>
       <c r="L25" s="28"/>
       <c r="M25" s="28"/>
-      <c r="N25" s="45"/>
-      <c r="O25" s="41"/>
+      <c r="N25" s="43"/>
+      <c r="O25" s="39"/>
       <c r="P25" s="28"/>
       <c r="Q25" s="28"/>
       <c r="R25" s="28"/>
@@ -2453,15 +2461,15 @@
       <c r="AP25" s="28"/>
       <c r="AQ25" s="28"/>
       <c r="AR25" s="28"/>
-      <c r="AS25" s="45"/>
-      <c r="AT25" s="41"/>
+      <c r="AS25" s="43"/>
+      <c r="AT25" s="39"/>
       <c r="AU25" s="28"/>
     </row>
     <row r="26" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="A26" s="34" t="s">
+      <c r="A26" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="B26" s="31"/>
+      <c r="B26" s="59"/>
       <c r="C26" s="26">
         <v>44184</v>
       </c>
@@ -2477,8 +2485,8 @@
       <c r="K26" s="28"/>
       <c r="L26" s="28"/>
       <c r="M26" s="28"/>
-      <c r="N26" s="45"/>
-      <c r="O26" s="41"/>
+      <c r="N26" s="43"/>
+      <c r="O26" s="39"/>
       <c r="P26" s="28"/>
       <c r="Q26" s="28"/>
       <c r="R26" s="28"/>
@@ -2508,15 +2516,15 @@
       <c r="AP26" s="28"/>
       <c r="AQ26" s="28"/>
       <c r="AR26" s="28"/>
-      <c r="AS26" s="45"/>
-      <c r="AT26" s="41"/>
+      <c r="AS26" s="43"/>
+      <c r="AT26" s="39"/>
       <c r="AU26" s="28"/>
     </row>
     <row r="27" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="A27" s="34" t="s">
+      <c r="A27" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="B27" s="31"/>
+      <c r="B27" s="59"/>
       <c r="C27" s="26">
         <v>44185</v>
       </c>
@@ -2532,8 +2540,8 @@
       <c r="K27" s="28"/>
       <c r="L27" s="28"/>
       <c r="M27" s="28"/>
-      <c r="N27" s="45"/>
-      <c r="O27" s="41"/>
+      <c r="N27" s="43"/>
+      <c r="O27" s="39"/>
       <c r="P27" s="28"/>
       <c r="Q27" s="28"/>
       <c r="R27" s="28"/>
@@ -2563,15 +2571,15 @@
       <c r="AP27" s="28"/>
       <c r="AQ27" s="28"/>
       <c r="AR27" s="28"/>
-      <c r="AS27" s="45"/>
-      <c r="AT27" s="41"/>
+      <c r="AS27" s="43"/>
+      <c r="AT27" s="39"/>
       <c r="AU27" s="28"/>
     </row>
     <row r="28" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="A28" s="34" t="s">
+      <c r="A28" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="B28" s="31"/>
+      <c r="B28" s="59"/>
       <c r="C28" s="26">
         <v>44185</v>
       </c>
@@ -2587,8 +2595,8 @@
       <c r="K28" s="28"/>
       <c r="L28" s="28"/>
       <c r="M28" s="28"/>
-      <c r="N28" s="45"/>
-      <c r="O28" s="41"/>
+      <c r="N28" s="43"/>
+      <c r="O28" s="39"/>
       <c r="P28" s="28"/>
       <c r="Q28" s="28"/>
       <c r="R28" s="28"/>
@@ -2618,15 +2626,15 @@
       <c r="AP28" s="28"/>
       <c r="AQ28" s="28"/>
       <c r="AR28" s="28"/>
-      <c r="AS28" s="45"/>
-      <c r="AT28" s="41"/>
+      <c r="AS28" s="43"/>
+      <c r="AT28" s="39"/>
       <c r="AU28" s="28"/>
     </row>
     <row r="29" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="A29" s="34" t="s">
+      <c r="A29" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="B29" s="31"/>
+      <c r="B29" s="59"/>
       <c r="C29" s="26">
         <v>44186</v>
       </c>
@@ -2642,8 +2650,8 @@
       <c r="K29" s="28"/>
       <c r="L29" s="28"/>
       <c r="M29" s="28"/>
-      <c r="N29" s="45"/>
-      <c r="O29" s="41"/>
+      <c r="N29" s="43"/>
+      <c r="O29" s="39"/>
       <c r="P29" s="28"/>
       <c r="Q29" s="28"/>
       <c r="R29" s="28"/>
@@ -2673,15 +2681,15 @@
       <c r="AP29" s="28"/>
       <c r="AQ29" s="28"/>
       <c r="AR29" s="28"/>
-      <c r="AS29" s="45"/>
-      <c r="AT29" s="41"/>
+      <c r="AS29" s="43"/>
+      <c r="AT29" s="39"/>
       <c r="AU29" s="28"/>
     </row>
     <row r="30" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="A30" s="34" t="s">
+      <c r="A30" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="B30" s="31"/>
+      <c r="B30" s="59"/>
       <c r="C30" s="26">
         <v>44187</v>
       </c>
@@ -2697,8 +2705,8 @@
       <c r="K30" s="28"/>
       <c r="L30" s="28"/>
       <c r="M30" s="28"/>
-      <c r="N30" s="45"/>
-      <c r="O30" s="41"/>
+      <c r="N30" s="43"/>
+      <c r="O30" s="39"/>
       <c r="P30" s="28"/>
       <c r="Q30" s="28"/>
       <c r="R30" s="28"/>
@@ -2728,15 +2736,15 @@
       <c r="AP30" s="28"/>
       <c r="AQ30" s="28"/>
       <c r="AR30" s="28"/>
-      <c r="AS30" s="45"/>
-      <c r="AT30" s="41"/>
+      <c r="AS30" s="43"/>
+      <c r="AT30" s="39"/>
       <c r="AU30" s="28"/>
     </row>
     <row r="31" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="A31" s="34" t="s">
+      <c r="A31" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="B31" s="31"/>
+      <c r="B31" s="59"/>
       <c r="C31" s="26">
         <v>44187</v>
       </c>
@@ -2752,8 +2760,8 @@
       <c r="K31" s="28"/>
       <c r="L31" s="28"/>
       <c r="M31" s="28"/>
-      <c r="N31" s="45"/>
-      <c r="O31" s="41"/>
+      <c r="N31" s="43"/>
+      <c r="O31" s="39"/>
       <c r="P31" s="28"/>
       <c r="Q31" s="28"/>
       <c r="R31" s="28"/>
@@ -2783,15 +2791,15 @@
       <c r="AP31" s="28"/>
       <c r="AQ31" s="28"/>
       <c r="AR31" s="28"/>
-      <c r="AS31" s="45"/>
-      <c r="AT31" s="41"/>
+      <c r="AS31" s="43"/>
+      <c r="AT31" s="39"/>
       <c r="AU31" s="28"/>
     </row>
     <row r="32" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="A32" s="34" t="s">
+      <c r="A32" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="B32" s="31"/>
+      <c r="B32" s="59"/>
       <c r="C32" s="26">
         <v>44187</v>
       </c>
@@ -2807,8 +2815,8 @@
       <c r="K32" s="28"/>
       <c r="L32" s="28"/>
       <c r="M32" s="28"/>
-      <c r="N32" s="45"/>
-      <c r="O32" s="41"/>
+      <c r="N32" s="43"/>
+      <c r="O32" s="39"/>
       <c r="P32" s="28"/>
       <c r="Q32" s="28"/>
       <c r="R32" s="28"/>
@@ -2838,15 +2846,15 @@
       <c r="AP32" s="28"/>
       <c r="AQ32" s="28"/>
       <c r="AR32" s="28"/>
-      <c r="AS32" s="45"/>
-      <c r="AT32" s="41"/>
+      <c r="AS32" s="43"/>
+      <c r="AT32" s="39"/>
       <c r="AU32" s="28"/>
     </row>
     <row r="33" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="A33" s="34" t="s">
+      <c r="A33" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="B33" s="31"/>
+      <c r="B33" s="59"/>
       <c r="C33" s="26">
         <v>44188</v>
       </c>
@@ -2862,8 +2870,8 @@
       <c r="K33" s="28"/>
       <c r="L33" s="28"/>
       <c r="M33" s="28"/>
-      <c r="N33" s="45"/>
-      <c r="O33" s="41"/>
+      <c r="N33" s="43"/>
+      <c r="O33" s="39"/>
       <c r="P33" s="28"/>
       <c r="Q33" s="28"/>
       <c r="R33" s="28"/>
@@ -2893,8 +2901,8 @@
       <c r="AP33" s="28"/>
       <c r="AQ33" s="28"/>
       <c r="AR33" s="28"/>
-      <c r="AS33" s="45"/>
-      <c r="AT33" s="41"/>
+      <c r="AS33" s="43"/>
+      <c r="AT33" s="39"/>
       <c r="AU33" s="28"/>
     </row>
     <row r="34" spans="1:47" x14ac:dyDescent="0.3">
@@ -2953,7 +2961,7 @@
       <c r="AU34" s="3"/>
     </row>
     <row r="35" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="A35" s="34" t="s">
+      <c r="A35" s="33" t="s">
         <v>33</v>
       </c>
       <c r="B35" s="28"/>
@@ -2972,8 +2980,8 @@
       <c r="K35" s="28"/>
       <c r="L35" s="28"/>
       <c r="M35" s="28"/>
-      <c r="N35" s="45"/>
-      <c r="O35" s="41"/>
+      <c r="N35" s="43"/>
+      <c r="O35" s="39"/>
       <c r="P35" s="28"/>
       <c r="Q35" s="28"/>
       <c r="R35" s="28"/>
@@ -3003,12 +3011,12 @@
       <c r="AP35" s="28"/>
       <c r="AQ35" s="28"/>
       <c r="AR35" s="28"/>
-      <c r="AS35" s="45"/>
-      <c r="AT35" s="41"/>
+      <c r="AS35" s="43"/>
+      <c r="AT35" s="39"/>
       <c r="AU35" s="28"/>
     </row>
     <row r="36" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="A36" s="34" t="s">
+      <c r="A36" s="33" t="s">
         <v>45</v>
       </c>
       <c r="B36" s="28"/>
@@ -3027,8 +3035,8 @@
       <c r="K36" s="28"/>
       <c r="L36" s="28"/>
       <c r="M36" s="28"/>
-      <c r="N36" s="45"/>
-      <c r="O36" s="41"/>
+      <c r="N36" s="43"/>
+      <c r="O36" s="39"/>
       <c r="P36" s="28"/>
       <c r="Q36" s="28"/>
       <c r="R36" s="28"/>
@@ -3058,12 +3066,12 @@
       <c r="AP36" s="28"/>
       <c r="AQ36" s="28"/>
       <c r="AR36" s="28"/>
-      <c r="AS36" s="45"/>
-      <c r="AT36" s="41"/>
+      <c r="AS36" s="43"/>
+      <c r="AT36" s="39"/>
       <c r="AU36" s="28"/>
     </row>
     <row r="37" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="A37" s="34" t="s">
+      <c r="A37" s="33" t="s">
         <v>46</v>
       </c>
       <c r="B37" s="28"/>
@@ -3082,8 +3090,8 @@
       <c r="K37" s="28"/>
       <c r="L37" s="28"/>
       <c r="M37" s="28"/>
-      <c r="N37" s="45"/>
-      <c r="O37" s="41"/>
+      <c r="N37" s="43"/>
+      <c r="O37" s="39"/>
       <c r="P37" s="28"/>
       <c r="Q37" s="28"/>
       <c r="R37" s="28"/>
@@ -3113,12 +3121,12 @@
       <c r="AP37" s="28"/>
       <c r="AQ37" s="28"/>
       <c r="AR37" s="28"/>
-      <c r="AS37" s="45"/>
-      <c r="AT37" s="41"/>
+      <c r="AS37" s="43"/>
+      <c r="AT37" s="39"/>
       <c r="AU37" s="28"/>
     </row>
     <row r="38" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="A38" s="34" t="s">
+      <c r="A38" s="33" t="s">
         <v>35</v>
       </c>
       <c r="B38" s="28"/>
@@ -3137,8 +3145,8 @@
       <c r="K38" s="28"/>
       <c r="L38" s="28"/>
       <c r="M38" s="28"/>
-      <c r="N38" s="45"/>
-      <c r="O38" s="41"/>
+      <c r="N38" s="43"/>
+      <c r="O38" s="39"/>
       <c r="P38" s="28"/>
       <c r="Q38" s="28"/>
       <c r="R38" s="28"/>
@@ -3168,12 +3176,12 @@
       <c r="AP38" s="27"/>
       <c r="AQ38" s="28"/>
       <c r="AR38" s="28"/>
-      <c r="AS38" s="45"/>
-      <c r="AT38" s="41"/>
+      <c r="AS38" s="43"/>
+      <c r="AT38" s="39"/>
       <c r="AU38" s="28"/>
     </row>
     <row r="39" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="A39" s="34" t="s">
+      <c r="A39" s="33" t="s">
         <v>47</v>
       </c>
       <c r="B39" s="28"/>
@@ -3192,8 +3200,8 @@
       <c r="K39" s="28"/>
       <c r="L39" s="28"/>
       <c r="M39" s="28"/>
-      <c r="N39" s="45"/>
-      <c r="O39" s="41"/>
+      <c r="N39" s="43"/>
+      <c r="O39" s="39"/>
       <c r="P39" s="28"/>
       <c r="Q39" s="28"/>
       <c r="R39" s="28"/>
@@ -3223,8 +3231,8 @@
       <c r="AP39" s="27"/>
       <c r="AQ39" s="28"/>
       <c r="AR39" s="28"/>
-      <c r="AS39" s="45"/>
-      <c r="AT39" s="41"/>
+      <c r="AS39" s="43"/>
+      <c r="AT39" s="39"/>
       <c r="AU39" s="28"/>
     </row>
     <row r="40" spans="1:47" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added project management page for admin
</commit_message>
<xml_diff>
--- a/Project_Plan.xlsx
+++ b/Project_Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1 UF\ResumeProjects\BugTracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD56BD14-5E6B-42CE-BFE8-50EC183719F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFA297BD-26AC-45FD-80D4-97455DB1EC72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{886EFED1-650A-4142-9A82-0722A0454DCF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="52">
   <si>
     <t>Project Manager</t>
   </si>
@@ -523,6 +523,9 @@
     <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -539,9 +542,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -882,10 +882,10 @@
   <dimension ref="A1:AU48"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="G15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="G21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="J28" sqref="J28"/>
+      <selection pane="bottomRight" activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -955,69 +955,69 @@
       <c r="D3" s="12"/>
       <c r="E3" s="12"/>
       <c r="F3" s="12"/>
-      <c r="G3" s="53" t="s">
+      <c r="G3" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="53"/>
-      <c r="I3" s="53"/>
-      <c r="J3" s="53"/>
-      <c r="K3" s="53"/>
-      <c r="L3" s="53"/>
-      <c r="M3" s="53"/>
-      <c r="N3" s="54"/>
-      <c r="O3" s="55" t="s">
+      <c r="H3" s="54"/>
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="54"/>
+      <c r="L3" s="54"/>
+      <c r="M3" s="54"/>
+      <c r="N3" s="55"/>
+      <c r="O3" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="P3" s="55"/>
-      <c r="Q3" s="55"/>
-      <c r="R3" s="55"/>
-      <c r="S3" s="55"/>
-      <c r="T3" s="55"/>
-      <c r="U3" s="55"/>
-      <c r="V3" s="55"/>
-      <c r="W3" s="55"/>
-      <c r="X3" s="55"/>
-      <c r="Y3" s="55"/>
-      <c r="Z3" s="55"/>
-      <c r="AA3" s="55"/>
-      <c r="AB3" s="55"/>
-      <c r="AC3" s="55"/>
-      <c r="AD3" s="55"/>
-      <c r="AE3" s="55"/>
-      <c r="AF3" s="55"/>
-      <c r="AG3" s="55"/>
-      <c r="AH3" s="55"/>
-      <c r="AI3" s="55"/>
-      <c r="AJ3" s="55"/>
-      <c r="AK3" s="55"/>
-      <c r="AL3" s="55"/>
-      <c r="AM3" s="55"/>
-      <c r="AN3" s="55"/>
-      <c r="AO3" s="55"/>
-      <c r="AP3" s="55"/>
-      <c r="AQ3" s="56"/>
-      <c r="AR3" s="56"/>
-      <c r="AS3" s="57"/>
-      <c r="AT3" s="55" t="s">
+      <c r="P3" s="56"/>
+      <c r="Q3" s="56"/>
+      <c r="R3" s="56"/>
+      <c r="S3" s="56"/>
+      <c r="T3" s="56"/>
+      <c r="U3" s="56"/>
+      <c r="V3" s="56"/>
+      <c r="W3" s="56"/>
+      <c r="X3" s="56"/>
+      <c r="Y3" s="56"/>
+      <c r="Z3" s="56"/>
+      <c r="AA3" s="56"/>
+      <c r="AB3" s="56"/>
+      <c r="AC3" s="56"/>
+      <c r="AD3" s="56"/>
+      <c r="AE3" s="56"/>
+      <c r="AF3" s="56"/>
+      <c r="AG3" s="56"/>
+      <c r="AH3" s="56"/>
+      <c r="AI3" s="56"/>
+      <c r="AJ3" s="56"/>
+      <c r="AK3" s="56"/>
+      <c r="AL3" s="56"/>
+      <c r="AM3" s="56"/>
+      <c r="AN3" s="56"/>
+      <c r="AO3" s="56"/>
+      <c r="AP3" s="56"/>
+      <c r="AQ3" s="57"/>
+      <c r="AR3" s="57"/>
+      <c r="AS3" s="58"/>
+      <c r="AT3" s="56" t="s">
         <v>49</v>
       </c>
-      <c r="AU3" s="55"/>
+      <c r="AU3" s="56"/>
     </row>
     <row r="4" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="A4" s="58" t="s">
+      <c r="A4" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="58" t="s">
+      <c r="B4" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="58" t="s">
+      <c r="C4" s="59" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="58"/>
-      <c r="E4" s="58" t="s">
+      <c r="D4" s="59"/>
+      <c r="E4" s="59" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="58"/>
+      <c r="F4" s="59"/>
       <c r="G4" s="48" t="s">
         <v>10</v>
       </c>
@@ -1143,8 +1143,8 @@
       </c>
     </row>
     <row r="5" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="A5" s="58"/>
-      <c r="B5" s="58"/>
+      <c r="A5" s="59"/>
+      <c r="B5" s="59"/>
       <c r="C5" s="13" t="s">
         <v>11</v>
       </c>
@@ -2302,7 +2302,7 @@
       <c r="A23" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="B23" s="59" t="s">
+      <c r="B23" s="53" t="s">
         <v>51</v>
       </c>
       <c r="C23" s="26">
@@ -2359,15 +2359,21 @@
       <c r="A24" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="59"/>
+      <c r="B24" s="53" t="s">
+        <v>23</v>
+      </c>
       <c r="C24" s="26">
         <v>44183</v>
       </c>
       <c r="D24" s="26">
         <v>44183</v>
       </c>
-      <c r="E24" s="26"/>
-      <c r="F24" s="26"/>
+      <c r="E24" s="26">
+        <v>44183</v>
+      </c>
+      <c r="F24" s="26">
+        <v>44183</v>
+      </c>
       <c r="G24" s="28"/>
       <c r="H24" s="28"/>
       <c r="I24" s="28"/>
@@ -2414,15 +2420,21 @@
       <c r="A25" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="B25" s="59"/>
+      <c r="B25" s="53" t="s">
+        <v>23</v>
+      </c>
       <c r="C25" s="26">
         <v>44184</v>
       </c>
       <c r="D25" s="26">
         <v>44184</v>
       </c>
-      <c r="E25" s="26"/>
-      <c r="F25" s="26"/>
+      <c r="E25" s="26">
+        <v>44183</v>
+      </c>
+      <c r="F25" s="26">
+        <v>44183</v>
+      </c>
       <c r="G25" s="28"/>
       <c r="H25" s="28"/>
       <c r="I25" s="28"/>
@@ -2469,15 +2481,21 @@
       <c r="A26" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="B26" s="59"/>
+      <c r="B26" s="53" t="s">
+        <v>23</v>
+      </c>
       <c r="C26" s="26">
         <v>44184</v>
       </c>
       <c r="D26" s="26">
         <v>44184</v>
       </c>
-      <c r="E26" s="26"/>
-      <c r="F26" s="26"/>
+      <c r="E26" s="26">
+        <v>44183</v>
+      </c>
+      <c r="F26" s="26">
+        <v>44183</v>
+      </c>
       <c r="G26" s="28"/>
       <c r="H26" s="28"/>
       <c r="I26" s="28"/>
@@ -2524,15 +2542,21 @@
       <c r="A27" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="B27" s="59"/>
+      <c r="B27" s="53" t="s">
+        <v>23</v>
+      </c>
       <c r="C27" s="26">
         <v>44185</v>
       </c>
       <c r="D27" s="26">
         <v>44185</v>
       </c>
-      <c r="E27" s="26"/>
-      <c r="F27" s="26"/>
+      <c r="E27" s="26">
+        <v>44183</v>
+      </c>
+      <c r="F27" s="26">
+        <v>44183</v>
+      </c>
       <c r="G27" s="28"/>
       <c r="H27" s="28"/>
       <c r="I27" s="28"/>
@@ -2579,15 +2603,21 @@
       <c r="A28" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="B28" s="59"/>
+      <c r="B28" s="53" t="s">
+        <v>23</v>
+      </c>
       <c r="C28" s="26">
         <v>44185</v>
       </c>
       <c r="D28" s="26">
         <v>44185</v>
       </c>
-      <c r="E28" s="26"/>
-      <c r="F28" s="26"/>
+      <c r="E28" s="26">
+        <v>44183</v>
+      </c>
+      <c r="F28" s="26">
+        <v>44183</v>
+      </c>
       <c r="G28" s="28"/>
       <c r="H28" s="28"/>
       <c r="I28" s="28"/>
@@ -2634,7 +2664,7 @@
       <c r="A29" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="B29" s="59"/>
+      <c r="B29" s="53"/>
       <c r="C29" s="26">
         <v>44186</v>
       </c>
@@ -2689,7 +2719,7 @@
       <c r="A30" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="B30" s="59"/>
+      <c r="B30" s="53"/>
       <c r="C30" s="26">
         <v>44187</v>
       </c>
@@ -2744,7 +2774,7 @@
       <c r="A31" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="B31" s="59"/>
+      <c r="B31" s="53"/>
       <c r="C31" s="26">
         <v>44187</v>
       </c>
@@ -2799,7 +2829,7 @@
       <c r="A32" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="B32" s="59"/>
+      <c r="B32" s="53"/>
       <c r="C32" s="26">
         <v>44187</v>
       </c>
@@ -2854,7 +2884,7 @@
       <c r="A33" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="B33" s="59"/>
+      <c r="B33" s="53"/>
       <c r="C33" s="26">
         <v>44188</v>
       </c>

</xml_diff>

<commit_message>
Added manager tickets and projects
</commit_message>
<xml_diff>
--- a/Project_Plan.xlsx
+++ b/Project_Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1 UF\ResumeProjects\BugTracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8320E028-5C51-489F-9C3C-4F35BAC50E60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7454F5C-B3EA-47A5-9528-43508B4F75CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{886EFED1-650A-4142-9A82-0722A0454DCF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="52">
   <si>
     <t>Project Manager</t>
   </si>
@@ -548,7 +548,47 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -882,10 +922,10 @@
   <dimension ref="A1:AU48"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="G21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="G32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="E31" sqref="E31"/>
+      <selection pane="bottomRight" activeCell="E39" sqref="E39:F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2664,7 +2704,9 @@
       <c r="A29" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="B29" s="53"/>
+      <c r="B29" s="53" t="s">
+        <v>23</v>
+      </c>
       <c r="C29" s="26">
         <v>44186</v>
       </c>
@@ -2674,7 +2716,9 @@
       <c r="E29" s="26">
         <v>44183</v>
       </c>
-      <c r="F29" s="26"/>
+      <c r="F29" s="26">
+        <v>44186</v>
+      </c>
       <c r="G29" s="28"/>
       <c r="H29" s="28"/>
       <c r="I29" s="28"/>
@@ -2721,7 +2765,9 @@
       <c r="A30" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="B30" s="53"/>
+      <c r="B30" s="53" t="s">
+        <v>23</v>
+      </c>
       <c r="C30" s="26">
         <v>44187</v>
       </c>
@@ -2731,7 +2777,9 @@
       <c r="E30" s="26">
         <v>44183</v>
       </c>
-      <c r="F30" s="26"/>
+      <c r="F30" s="26">
+        <v>44186</v>
+      </c>
       <c r="G30" s="28"/>
       <c r="H30" s="28"/>
       <c r="I30" s="28"/>
@@ -2778,15 +2826,21 @@
       <c r="A31" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="B31" s="53"/>
+      <c r="B31" s="53" t="s">
+        <v>23</v>
+      </c>
       <c r="C31" s="26">
         <v>44187</v>
       </c>
       <c r="D31" s="26">
         <v>44187</v>
       </c>
-      <c r="E31" s="26"/>
-      <c r="F31" s="26"/>
+      <c r="E31" s="26">
+        <v>44186</v>
+      </c>
+      <c r="F31" s="26">
+        <v>44186</v>
+      </c>
       <c r="G31" s="28"/>
       <c r="H31" s="28"/>
       <c r="I31" s="28"/>
@@ -2833,15 +2887,21 @@
       <c r="A32" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="B32" s="53"/>
+      <c r="B32" s="53" t="s">
+        <v>23</v>
+      </c>
       <c r="C32" s="26">
         <v>44187</v>
       </c>
       <c r="D32" s="26">
         <v>44187</v>
       </c>
-      <c r="E32" s="26"/>
-      <c r="F32" s="26"/>
+      <c r="E32" s="26">
+        <v>44186</v>
+      </c>
+      <c r="F32" s="26">
+        <v>44186</v>
+      </c>
       <c r="G32" s="28"/>
       <c r="H32" s="28"/>
       <c r="I32" s="28"/>
@@ -2888,15 +2948,21 @@
       <c r="A33" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="B33" s="53"/>
+      <c r="B33" s="53" t="s">
+        <v>23</v>
+      </c>
       <c r="C33" s="26">
         <v>44188</v>
       </c>
       <c r="D33" s="26">
         <v>44188</v>
       </c>
-      <c r="E33" s="26"/>
-      <c r="F33" s="26"/>
+      <c r="E33" s="26">
+        <v>44186</v>
+      </c>
+      <c r="F33" s="26">
+        <v>44186</v>
+      </c>
       <c r="G33" s="28"/>
       <c r="H33" s="28"/>
       <c r="I33" s="28"/>
@@ -3053,15 +3119,21 @@
       <c r="A36" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="B36" s="28"/>
+      <c r="B36" s="53" t="s">
+        <v>23</v>
+      </c>
       <c r="C36" s="26">
         <v>44192</v>
       </c>
       <c r="D36" s="26">
         <v>44192</v>
       </c>
-      <c r="E36" s="26"/>
-      <c r="F36" s="26"/>
+      <c r="E36" s="26">
+        <v>44186</v>
+      </c>
+      <c r="F36" s="26">
+        <v>44186</v>
+      </c>
       <c r="G36" s="28"/>
       <c r="H36" s="28"/>
       <c r="I36" s="28"/>
@@ -3108,15 +3180,21 @@
       <c r="A37" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="B37" s="28"/>
+      <c r="B37" s="53" t="s">
+        <v>23</v>
+      </c>
       <c r="C37" s="26">
         <v>44192</v>
       </c>
       <c r="D37" s="26">
         <v>44192</v>
       </c>
-      <c r="E37" s="26"/>
-      <c r="F37" s="26"/>
+      <c r="E37" s="26">
+        <v>44186</v>
+      </c>
+      <c r="F37" s="26">
+        <v>44186</v>
+      </c>
       <c r="G37" s="28"/>
       <c r="H37" s="28"/>
       <c r="I37" s="28"/>
@@ -3163,15 +3241,21 @@
       <c r="A38" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="B38" s="28"/>
+      <c r="B38" s="53" t="s">
+        <v>23</v>
+      </c>
       <c r="C38" s="26">
         <v>44193</v>
       </c>
       <c r="D38" s="26">
         <v>44193</v>
       </c>
-      <c r="E38" s="26"/>
-      <c r="F38" s="26"/>
+      <c r="E38" s="26">
+        <v>44186</v>
+      </c>
+      <c r="F38" s="26">
+        <v>44186</v>
+      </c>
       <c r="G38" s="28"/>
       <c r="H38" s="28"/>
       <c r="I38" s="28"/>
@@ -3218,15 +3302,21 @@
       <c r="A39" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="B39" s="28"/>
+      <c r="B39" s="53" t="s">
+        <v>23</v>
+      </c>
       <c r="C39" s="26">
         <v>44193</v>
       </c>
       <c r="D39" s="26">
         <v>44193</v>
       </c>
-      <c r="E39" s="26"/>
-      <c r="F39" s="26"/>
+      <c r="E39" s="26">
+        <v>44186</v>
+      </c>
+      <c r="F39" s="26">
+        <v>44186</v>
+      </c>
       <c r="G39" s="28"/>
       <c r="H39" s="28"/>
       <c r="I39" s="28"/>
@@ -3448,11 +3538,31 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A40:AP40 B6:B34">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+      <formula>"Complete"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AT40:AU40">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+      <formula>"Complete"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B36">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+      <formula>"Complete"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B37">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>"Complete"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B39">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Complete"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AT40:AU40">
+  <conditionalFormatting sqref="B38">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Complete"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Added view images to readme
</commit_message>
<xml_diff>
--- a/Project_Plan.xlsx
+++ b/Project_Plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1 UF\ResumeProjects\BugTracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66942122-A3C5-4070-967F-6F009920928D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93FCD59E-CD1E-4E2C-BFD8-AA6A59D85374}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{886EFED1-650A-4142-9A82-0722A0454DCF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{886EFED1-650A-4142-9A82-0722A0454DCF}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="51">
   <si>
     <t>Project Manager</t>
   </si>
@@ -93,9 +93,6 @@
     <t>Name :</t>
   </si>
   <si>
-    <t>Bug Tracker</t>
-  </si>
-  <si>
     <t>Setup</t>
   </si>
   <si>
@@ -189,7 +186,7 @@
     <t>1. view : login page setup</t>
   </si>
   <si>
-    <t>removed</t>
+    <t>Bug Trac</t>
   </si>
 </sst>
 </file>
@@ -929,13 +926,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{174427EE-9525-4626-99D7-0EF4B41F1E97}">
-  <dimension ref="A1:AU48"/>
+  <dimension ref="A1:AU47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="G32" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
+      <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="F36" sqref="F36"/>
+      <selection pane="bottomRight" activeCell="AZ25" sqref="AZ25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -991,7 +988,7 @@
         <v>18</v>
       </c>
       <c r="B1" s="46" t="s">
-        <v>19</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:47" ht="3.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -1006,7 +1003,7 @@
       <c r="E3" s="12"/>
       <c r="F3" s="12"/>
       <c r="G3" s="54" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H3" s="54"/>
       <c r="I3" s="54"/>
@@ -1016,7 +1013,7 @@
       <c r="M3" s="54"/>
       <c r="N3" s="55"/>
       <c r="O3" s="56" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P3" s="56"/>
       <c r="Q3" s="56"/>
@@ -1049,7 +1046,7 @@
       <c r="AR3" s="57"/>
       <c r="AS3" s="58"/>
       <c r="AT3" s="56" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AU3" s="56"/>
     </row>
@@ -1333,10 +1330,10 @@
     </row>
     <row r="6" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6" s="14">
         <v>44158</v>
@@ -1394,10 +1391,10 @@
     </row>
     <row r="7" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A7" s="34" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" s="26">
         <v>44158</v>
@@ -1510,10 +1507,10 @@
     </row>
     <row r="9" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A9" s="33" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" s="26">
         <v>44159</v>
@@ -1571,10 +1568,10 @@
     </row>
     <row r="10" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A10" s="33" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10" s="26">
         <v>44160</v>
@@ -1632,10 +1629,10 @@
     </row>
     <row r="11" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A11" s="33" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C11" s="26">
         <v>44174</v>
@@ -1693,10 +1690,10 @@
     </row>
     <row r="12" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A12" s="33" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" s="26">
         <v>44176</v>
@@ -1813,10 +1810,10 @@
     </row>
     <row r="14" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A14" s="47" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C14" s="35">
         <v>44162</v>
@@ -1929,10 +1926,10 @@
     </row>
     <row r="16" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A16" s="33" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C16" s="26">
         <v>44165</v>
@@ -1990,10 +1987,10 @@
     </row>
     <row r="17" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A17" s="33" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C17" s="26">
         <v>44165</v>
@@ -2051,10 +2048,10 @@
     </row>
     <row r="18" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A18" s="33" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B18" s="25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C18" s="26">
         <v>44166</v>
@@ -2112,10 +2109,10 @@
     </row>
     <row r="19" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A19" s="33" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B19" s="25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C19" s="26">
         <v>44169</v>
@@ -2173,10 +2170,10 @@
     </row>
     <row r="20" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A20" s="33" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C20" s="26">
         <v>44171</v>
@@ -2234,10 +2231,10 @@
     </row>
     <row r="21" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A21" s="33" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C21" s="26">
         <v>44176</v>
@@ -2295,7 +2292,7 @@
     </row>
     <row r="22" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22" s="11"/>
       <c r="C22" s="10">
@@ -2353,7 +2350,7 @@
         <v>33</v>
       </c>
       <c r="B23" s="53" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="C23" s="26">
         <v>44183</v>
@@ -2361,8 +2358,12 @@
       <c r="D23" s="26">
         <v>44183</v>
       </c>
-      <c r="E23" s="26"/>
-      <c r="F23" s="26"/>
+      <c r="E23" s="26">
+        <v>44183</v>
+      </c>
+      <c r="F23" s="26">
+        <v>44183</v>
+      </c>
       <c r="G23" s="28"/>
       <c r="H23" s="28"/>
       <c r="I23" s="28"/>
@@ -2407,16 +2408,16 @@
     </row>
     <row r="24" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A24" s="33" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B24" s="53" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C24" s="26">
-        <v>44183</v>
+        <v>44184</v>
       </c>
       <c r="D24" s="26">
-        <v>44183</v>
+        <v>44184</v>
       </c>
       <c r="E24" s="26">
         <v>44183</v>
@@ -2449,8 +2450,8 @@
       <c r="AC24" s="28"/>
       <c r="AD24" s="28"/>
       <c r="AE24" s="28"/>
-      <c r="AF24" s="27"/>
-      <c r="AG24" s="28"/>
+      <c r="AF24" s="28"/>
+      <c r="AG24" s="27"/>
       <c r="AH24" s="28"/>
       <c r="AI24" s="28"/>
       <c r="AJ24" s="28"/>
@@ -2471,7 +2472,7 @@
         <v>38</v>
       </c>
       <c r="B25" s="53" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C25" s="26">
         <v>44184</v>
@@ -2529,16 +2530,16 @@
     </row>
     <row r="26" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A26" s="33" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B26" s="53" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C26" s="26">
-        <v>44184</v>
+        <v>44185</v>
       </c>
       <c r="D26" s="26">
-        <v>44184</v>
+        <v>44185</v>
       </c>
       <c r="E26" s="26">
         <v>44183</v>
@@ -2572,8 +2573,8 @@
       <c r="AD26" s="28"/>
       <c r="AE26" s="28"/>
       <c r="AF26" s="28"/>
-      <c r="AG26" s="27"/>
-      <c r="AH26" s="28"/>
+      <c r="AG26" s="28"/>
+      <c r="AH26" s="27"/>
       <c r="AI26" s="28"/>
       <c r="AJ26" s="28"/>
       <c r="AK26" s="28"/>
@@ -2593,7 +2594,7 @@
         <v>36</v>
       </c>
       <c r="B27" s="53" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C27" s="26">
         <v>44185</v>
@@ -2651,22 +2652,22 @@
     </row>
     <row r="28" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A28" s="33" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B28" s="53" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C28" s="26">
-        <v>44185</v>
+        <v>44186</v>
       </c>
       <c r="D28" s="26">
-        <v>44185</v>
+        <v>44186</v>
       </c>
       <c r="E28" s="26">
         <v>44183</v>
       </c>
       <c r="F28" s="26">
-        <v>44183</v>
+        <v>44186</v>
       </c>
       <c r="G28" s="28"/>
       <c r="H28" s="28"/>
@@ -2695,8 +2696,8 @@
       <c r="AE28" s="28"/>
       <c r="AF28" s="28"/>
       <c r="AG28" s="28"/>
-      <c r="AH28" s="27"/>
-      <c r="AI28" s="28"/>
+      <c r="AH28" s="28"/>
+      <c r="AI28" s="27"/>
       <c r="AJ28" s="28"/>
       <c r="AK28" s="28"/>
       <c r="AL28" s="28"/>
@@ -2715,13 +2716,13 @@
         <v>40</v>
       </c>
       <c r="B29" s="53" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C29" s="26">
-        <v>44186</v>
+        <v>44187</v>
       </c>
       <c r="D29" s="26">
-        <v>44186</v>
+        <v>44187</v>
       </c>
       <c r="E29" s="26">
         <v>44183</v>
@@ -2757,8 +2758,8 @@
       <c r="AF29" s="28"/>
       <c r="AG29" s="28"/>
       <c r="AH29" s="28"/>
-      <c r="AI29" s="27"/>
-      <c r="AJ29" s="28"/>
+      <c r="AI29" s="28"/>
+      <c r="AJ29" s="27"/>
       <c r="AK29" s="28"/>
       <c r="AL29" s="28"/>
       <c r="AM29" s="28"/>
@@ -2776,7 +2777,7 @@
         <v>41</v>
       </c>
       <c r="B30" s="53" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C30" s="26">
         <v>44187</v>
@@ -2785,7 +2786,7 @@
         <v>44187</v>
       </c>
       <c r="E30" s="26">
-        <v>44183</v>
+        <v>44186</v>
       </c>
       <c r="F30" s="26">
         <v>44186</v>
@@ -2837,7 +2838,7 @@
         <v>42</v>
       </c>
       <c r="B31" s="53" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C31" s="26">
         <v>44187</v>
@@ -2898,13 +2899,13 @@
         <v>43</v>
       </c>
       <c r="B32" s="53" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C32" s="26">
-        <v>44187</v>
+        <v>44188</v>
       </c>
       <c r="D32" s="26">
-        <v>44187</v>
+        <v>44188</v>
       </c>
       <c r="E32" s="26">
         <v>44186</v>
@@ -2941,8 +2942,8 @@
       <c r="AG32" s="28"/>
       <c r="AH32" s="28"/>
       <c r="AI32" s="28"/>
-      <c r="AJ32" s="27"/>
-      <c r="AK32" s="28"/>
+      <c r="AJ32" s="28"/>
+      <c r="AK32" s="27"/>
       <c r="AL32" s="28"/>
       <c r="AM32" s="28"/>
       <c r="AN32" s="28"/>
@@ -2955,139 +2956,139 @@
       <c r="AU32" s="28"/>
     </row>
     <row r="33" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="A33" s="33" t="s">
-        <v>44</v>
-      </c>
-      <c r="B33" s="53" t="s">
-        <v>23</v>
-      </c>
-      <c r="C33" s="26">
-        <v>44188</v>
-      </c>
-      <c r="D33" s="26">
-        <v>44188</v>
-      </c>
-      <c r="E33" s="26">
-        <v>44186</v>
-      </c>
-      <c r="F33" s="26">
-        <v>44186</v>
-      </c>
-      <c r="G33" s="28"/>
-      <c r="H33" s="28"/>
-      <c r="I33" s="28"/>
-      <c r="J33" s="28"/>
-      <c r="K33" s="28"/>
-      <c r="L33" s="28"/>
-      <c r="M33" s="28"/>
-      <c r="N33" s="43"/>
-      <c r="O33" s="39"/>
-      <c r="P33" s="28"/>
-      <c r="Q33" s="28"/>
-      <c r="R33" s="28"/>
-      <c r="S33" s="28"/>
-      <c r="T33" s="28"/>
-      <c r="U33" s="28"/>
-      <c r="V33" s="28"/>
-      <c r="W33" s="28"/>
-      <c r="X33" s="28"/>
-      <c r="Y33" s="28"/>
-      <c r="Z33" s="28"/>
-      <c r="AA33" s="28"/>
-      <c r="AB33" s="28"/>
-      <c r="AC33" s="28"/>
-      <c r="AD33" s="28"/>
-      <c r="AE33" s="28"/>
-      <c r="AF33" s="28"/>
-      <c r="AG33" s="28"/>
-      <c r="AH33" s="28"/>
-      <c r="AI33" s="28"/>
-      <c r="AJ33" s="28"/>
-      <c r="AK33" s="27"/>
-      <c r="AL33" s="28"/>
-      <c r="AM33" s="28"/>
-      <c r="AN33" s="28"/>
-      <c r="AO33" s="28"/>
-      <c r="AP33" s="28"/>
-      <c r="AQ33" s="28"/>
-      <c r="AR33" s="28"/>
-      <c r="AS33" s="43"/>
-      <c r="AT33" s="39"/>
-      <c r="AU33" s="28"/>
+      <c r="A33" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" s="11"/>
+      <c r="C33" s="10">
+        <v>44189</v>
+      </c>
+      <c r="D33" s="10">
+        <v>44193</v>
+      </c>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
+      <c r="M33" s="3"/>
+      <c r="N33" s="17"/>
+      <c r="O33" s="3"/>
+      <c r="P33" s="3"/>
+      <c r="Q33" s="3"/>
+      <c r="R33" s="3"/>
+      <c r="S33" s="3"/>
+      <c r="T33" s="3"/>
+      <c r="U33" s="3"/>
+      <c r="V33" s="3"/>
+      <c r="W33" s="3"/>
+      <c r="X33" s="3"/>
+      <c r="Y33" s="3"/>
+      <c r="Z33" s="3"/>
+      <c r="AA33" s="3"/>
+      <c r="AB33" s="3"/>
+      <c r="AC33" s="3"/>
+      <c r="AD33" s="3"/>
+      <c r="AE33" s="3"/>
+      <c r="AF33" s="3"/>
+      <c r="AG33" s="3"/>
+      <c r="AH33" s="3"/>
+      <c r="AI33" s="3"/>
+      <c r="AJ33" s="3"/>
+      <c r="AK33" s="3"/>
+      <c r="AL33" s="5"/>
+      <c r="AM33" s="5"/>
+      <c r="AN33" s="5"/>
+      <c r="AO33" s="5"/>
+      <c r="AP33" s="5"/>
+      <c r="AQ33" s="3"/>
+      <c r="AR33" s="3"/>
+      <c r="AS33" s="17"/>
+      <c r="AT33" s="3"/>
+      <c r="AU33" s="3"/>
     </row>
     <row r="34" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="A34" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B34" s="11"/>
-      <c r="C34" s="10">
+      <c r="A34" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34" s="53" t="s">
+        <v>22</v>
+      </c>
+      <c r="C34" s="26">
         <v>44189</v>
       </c>
-      <c r="D34" s="10">
-        <v>44193</v>
-      </c>
-      <c r="E34" s="11"/>
-      <c r="F34" s="11"/>
-      <c r="G34" s="3"/>
-      <c r="H34" s="3"/>
-      <c r="I34" s="3"/>
-      <c r="J34" s="3"/>
-      <c r="K34" s="3"/>
-      <c r="L34" s="3"/>
-      <c r="M34" s="3"/>
-      <c r="N34" s="17"/>
-      <c r="O34" s="3"/>
-      <c r="P34" s="3"/>
-      <c r="Q34" s="3"/>
-      <c r="R34" s="3"/>
-      <c r="S34" s="3"/>
-      <c r="T34" s="3"/>
-      <c r="U34" s="3"/>
-      <c r="V34" s="3"/>
-      <c r="W34" s="3"/>
-      <c r="X34" s="3"/>
-      <c r="Y34" s="3"/>
-      <c r="Z34" s="3"/>
-      <c r="AA34" s="3"/>
-      <c r="AB34" s="3"/>
-      <c r="AC34" s="3"/>
-      <c r="AD34" s="3"/>
-      <c r="AE34" s="3"/>
-      <c r="AF34" s="3"/>
-      <c r="AG34" s="3"/>
-      <c r="AH34" s="3"/>
-      <c r="AI34" s="3"/>
-      <c r="AJ34" s="3"/>
-      <c r="AK34" s="3"/>
-      <c r="AL34" s="5"/>
-      <c r="AM34" s="5"/>
-      <c r="AN34" s="5"/>
-      <c r="AO34" s="5"/>
-      <c r="AP34" s="5"/>
-      <c r="AQ34" s="3"/>
-      <c r="AR34" s="3"/>
-      <c r="AS34" s="17"/>
-      <c r="AT34" s="3"/>
-      <c r="AU34" s="3"/>
+      <c r="D34" s="26">
+        <v>44191</v>
+      </c>
+      <c r="E34" s="26">
+        <v>44190</v>
+      </c>
+      <c r="F34" s="26">
+        <v>44191</v>
+      </c>
+      <c r="G34" s="28"/>
+      <c r="H34" s="28"/>
+      <c r="I34" s="28"/>
+      <c r="J34" s="28"/>
+      <c r="K34" s="28"/>
+      <c r="L34" s="28"/>
+      <c r="M34" s="28"/>
+      <c r="N34" s="43"/>
+      <c r="O34" s="39"/>
+      <c r="P34" s="28"/>
+      <c r="Q34" s="28"/>
+      <c r="R34" s="28"/>
+      <c r="S34" s="28"/>
+      <c r="T34" s="28"/>
+      <c r="U34" s="28"/>
+      <c r="V34" s="28"/>
+      <c r="W34" s="28"/>
+      <c r="X34" s="28"/>
+      <c r="Y34" s="28"/>
+      <c r="Z34" s="28"/>
+      <c r="AA34" s="28"/>
+      <c r="AB34" s="28"/>
+      <c r="AC34" s="28"/>
+      <c r="AD34" s="28"/>
+      <c r="AE34" s="28"/>
+      <c r="AF34" s="28"/>
+      <c r="AG34" s="28"/>
+      <c r="AH34" s="28"/>
+      <c r="AI34" s="28"/>
+      <c r="AJ34" s="28"/>
+      <c r="AK34" s="28"/>
+      <c r="AL34" s="27"/>
+      <c r="AM34" s="27"/>
+      <c r="AN34" s="27"/>
+      <c r="AO34" s="28"/>
+      <c r="AP34" s="28"/>
+      <c r="AQ34" s="28"/>
+      <c r="AR34" s="28"/>
+      <c r="AS34" s="43"/>
+      <c r="AT34" s="39"/>
+      <c r="AU34" s="28"/>
     </row>
     <row r="35" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A35" s="33" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="B35" s="53" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C35" s="26">
-        <v>44189</v>
+        <v>44192</v>
       </c>
       <c r="D35" s="26">
-        <v>44191</v>
+        <v>44192</v>
       </c>
       <c r="E35" s="26">
-        <v>44190</v>
+        <v>44186</v>
       </c>
       <c r="F35" s="26">
-        <v>44191</v>
+        <v>44186</v>
       </c>
       <c r="G35" s="28"/>
       <c r="H35" s="28"/>
@@ -3120,10 +3121,10 @@
       <c r="AI35" s="28"/>
       <c r="AJ35" s="28"/>
       <c r="AK35" s="28"/>
-      <c r="AL35" s="27"/>
-      <c r="AM35" s="27"/>
-      <c r="AN35" s="27"/>
-      <c r="AO35" s="28"/>
+      <c r="AL35" s="28"/>
+      <c r="AM35" s="28"/>
+      <c r="AN35" s="28"/>
+      <c r="AO35" s="27"/>
       <c r="AP35" s="28"/>
       <c r="AQ35" s="28"/>
       <c r="AR35" s="28"/>
@@ -3136,7 +3137,7 @@
         <v>45</v>
       </c>
       <c r="B36" s="53" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C36" s="26">
         <v>44192</v>
@@ -3194,16 +3195,16 @@
     </row>
     <row r="37" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A37" s="33" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="B37" s="53" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C37" s="26">
-        <v>44192</v>
+        <v>44193</v>
       </c>
       <c r="D37" s="26">
-        <v>44192</v>
+        <v>44193</v>
       </c>
       <c r="E37" s="26">
         <v>44186</v>
@@ -3245,8 +3246,8 @@
       <c r="AL37" s="28"/>
       <c r="AM37" s="28"/>
       <c r="AN37" s="28"/>
-      <c r="AO37" s="27"/>
-      <c r="AP37" s="28"/>
+      <c r="AO37" s="28"/>
+      <c r="AP37" s="27"/>
       <c r="AQ37" s="28"/>
       <c r="AR37" s="28"/>
       <c r="AS37" s="43"/>
@@ -3255,10 +3256,10 @@
     </row>
     <row r="38" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A38" s="33" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="B38" s="53" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C38" s="26">
         <v>44193</v>
@@ -3315,175 +3316,124 @@
       <c r="AU38" s="28"/>
     </row>
     <row r="39" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="A39" s="33" t="s">
+      <c r="A39" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B39" s="53" t="s">
-        <v>23</v>
-      </c>
-      <c r="C39" s="26">
-        <v>44193</v>
-      </c>
-      <c r="D39" s="26">
-        <v>44193</v>
-      </c>
-      <c r="E39" s="26">
-        <v>44186</v>
-      </c>
-      <c r="F39" s="26">
-        <v>44186</v>
-      </c>
-      <c r="G39" s="28"/>
-      <c r="H39" s="28"/>
-      <c r="I39" s="28"/>
-      <c r="J39" s="28"/>
-      <c r="K39" s="28"/>
-      <c r="L39" s="28"/>
-      <c r="M39" s="28"/>
-      <c r="N39" s="43"/>
-      <c r="O39" s="39"/>
-      <c r="P39" s="28"/>
-      <c r="Q39" s="28"/>
-      <c r="R39" s="28"/>
-      <c r="S39" s="28"/>
-      <c r="T39" s="28"/>
-      <c r="U39" s="28"/>
-      <c r="V39" s="28"/>
-      <c r="W39" s="28"/>
-      <c r="X39" s="28"/>
-      <c r="Y39" s="28"/>
-      <c r="Z39" s="28"/>
-      <c r="AA39" s="28"/>
-      <c r="AB39" s="28"/>
-      <c r="AC39" s="28"/>
-      <c r="AD39" s="28"/>
-      <c r="AE39" s="28"/>
-      <c r="AF39" s="28"/>
-      <c r="AG39" s="28"/>
-      <c r="AH39" s="28"/>
-      <c r="AI39" s="28"/>
-      <c r="AJ39" s="28"/>
-      <c r="AK39" s="28"/>
-      <c r="AL39" s="28"/>
-      <c r="AM39" s="28"/>
-      <c r="AN39" s="28"/>
-      <c r="AO39" s="28"/>
-      <c r="AP39" s="27"/>
-      <c r="AQ39" s="28"/>
-      <c r="AR39" s="28"/>
-      <c r="AS39" s="43"/>
-      <c r="AT39" s="39"/>
-      <c r="AU39" s="28"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="10">
+        <v>44194</v>
+      </c>
+      <c r="D39" s="10">
+        <v>44195</v>
+      </c>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11"/>
+      <c r="H39" s="11"/>
+      <c r="I39" s="11"/>
+      <c r="J39" s="11"/>
+      <c r="K39" s="11"/>
+      <c r="L39" s="11"/>
+      <c r="M39" s="11"/>
+      <c r="N39" s="18"/>
+      <c r="O39" s="11"/>
+      <c r="P39" s="11"/>
+      <c r="Q39" s="11"/>
+      <c r="R39" s="11"/>
+      <c r="S39" s="11"/>
+      <c r="T39" s="11"/>
+      <c r="U39" s="11"/>
+      <c r="V39" s="11"/>
+      <c r="W39" s="11"/>
+      <c r="X39" s="11"/>
+      <c r="Y39" s="11"/>
+      <c r="Z39" s="11"/>
+      <c r="AA39" s="11"/>
+      <c r="AB39" s="11"/>
+      <c r="AC39" s="11"/>
+      <c r="AD39" s="11"/>
+      <c r="AE39" s="11"/>
+      <c r="AF39" s="11"/>
+      <c r="AG39" s="11"/>
+      <c r="AH39" s="11"/>
+      <c r="AI39" s="11"/>
+      <c r="AJ39" s="11"/>
+      <c r="AK39" s="11"/>
+      <c r="AL39" s="11"/>
+      <c r="AM39" s="11"/>
+      <c r="AN39" s="11"/>
+      <c r="AO39" s="11"/>
+      <c r="AP39" s="11"/>
+      <c r="AQ39" s="5"/>
+      <c r="AR39" s="5"/>
+      <c r="AS39" s="17"/>
+      <c r="AT39" s="11"/>
+      <c r="AU39" s="11"/>
     </row>
     <row r="40" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="A40" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B40" s="11"/>
-      <c r="C40" s="10">
-        <v>44194</v>
-      </c>
-      <c r="D40" s="10">
-        <v>44195</v>
-      </c>
-      <c r="E40" s="11"/>
-      <c r="F40" s="11"/>
-      <c r="G40" s="11"/>
-      <c r="H40" s="11"/>
-      <c r="I40" s="11"/>
-      <c r="J40" s="11"/>
-      <c r="K40" s="11"/>
-      <c r="L40" s="11"/>
-      <c r="M40" s="11"/>
-      <c r="N40" s="18"/>
-      <c r="O40" s="11"/>
-      <c r="P40" s="11"/>
-      <c r="Q40" s="11"/>
-      <c r="R40" s="11"/>
-      <c r="S40" s="11"/>
-      <c r="T40" s="11"/>
-      <c r="U40" s="11"/>
-      <c r="V40" s="11"/>
-      <c r="W40" s="11"/>
-      <c r="X40" s="11"/>
-      <c r="Y40" s="11"/>
-      <c r="Z40" s="11"/>
-      <c r="AA40" s="11"/>
-      <c r="AB40" s="11"/>
-      <c r="AC40" s="11"/>
-      <c r="AD40" s="11"/>
-      <c r="AE40" s="11"/>
-      <c r="AF40" s="11"/>
-      <c r="AG40" s="11"/>
-      <c r="AH40" s="11"/>
-      <c r="AI40" s="11"/>
-      <c r="AJ40" s="11"/>
-      <c r="AK40" s="11"/>
-      <c r="AL40" s="11"/>
-      <c r="AM40" s="11"/>
-      <c r="AN40" s="11"/>
-      <c r="AO40" s="11"/>
-      <c r="AP40" s="11"/>
-      <c r="AQ40" s="5"/>
-      <c r="AR40" s="5"/>
-      <c r="AS40" s="17"/>
-      <c r="AT40" s="11"/>
-      <c r="AU40" s="11"/>
+      <c r="A40" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B40" s="20"/>
+      <c r="C40" s="23">
+        <v>43831</v>
+      </c>
+      <c r="D40" s="23">
+        <v>43832</v>
+      </c>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
+      <c r="H40" s="20"/>
+      <c r="I40" s="20"/>
+      <c r="J40" s="20"/>
+      <c r="K40" s="20"/>
+      <c r="L40" s="20"/>
+      <c r="M40" s="20"/>
+      <c r="N40" s="21"/>
+      <c r="O40" s="20"/>
+      <c r="P40" s="20"/>
+      <c r="Q40" s="20"/>
+      <c r="R40" s="20"/>
+      <c r="S40" s="20"/>
+      <c r="T40" s="20"/>
+      <c r="U40" s="20"/>
+      <c r="V40" s="20"/>
+      <c r="W40" s="20"/>
+      <c r="X40" s="20"/>
+      <c r="Y40" s="20"/>
+      <c r="Z40" s="20"/>
+      <c r="AA40" s="20"/>
+      <c r="AB40" s="20"/>
+      <c r="AC40" s="20"/>
+      <c r="AD40" s="20"/>
+      <c r="AE40" s="20"/>
+      <c r="AF40" s="20"/>
+      <c r="AG40" s="20"/>
+      <c r="AH40" s="20"/>
+      <c r="AI40" s="20"/>
+      <c r="AJ40" s="20"/>
+      <c r="AK40" s="20"/>
+      <c r="AL40" s="20"/>
+      <c r="AM40" s="20"/>
+      <c r="AN40" s="20"/>
+      <c r="AO40" s="20"/>
+      <c r="AP40" s="20"/>
+      <c r="AQ40" s="20"/>
+      <c r="AR40" s="20"/>
+      <c r="AS40" s="21"/>
+      <c r="AT40" s="22"/>
+      <c r="AU40" s="22"/>
     </row>
     <row r="41" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="A41" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B41" s="20"/>
-      <c r="C41" s="23">
-        <v>43831</v>
-      </c>
-      <c r="D41" s="23">
-        <v>43832</v>
-      </c>
-      <c r="E41" s="20"/>
-      <c r="F41" s="20"/>
-      <c r="G41" s="20"/>
-      <c r="H41" s="20"/>
-      <c r="I41" s="20"/>
-      <c r="J41" s="20"/>
-      <c r="K41" s="20"/>
-      <c r="L41" s="20"/>
-      <c r="M41" s="20"/>
-      <c r="N41" s="21"/>
-      <c r="O41" s="20"/>
-      <c r="P41" s="20"/>
-      <c r="Q41" s="20"/>
-      <c r="R41" s="20"/>
-      <c r="S41" s="20"/>
-      <c r="T41" s="20"/>
-      <c r="U41" s="20"/>
-      <c r="V41" s="20"/>
-      <c r="W41" s="20"/>
-      <c r="X41" s="20"/>
-      <c r="Y41" s="20"/>
-      <c r="Z41" s="20"/>
-      <c r="AA41" s="20"/>
-      <c r="AB41" s="20"/>
-      <c r="AC41" s="20"/>
-      <c r="AD41" s="20"/>
-      <c r="AE41" s="20"/>
-      <c r="AF41" s="20"/>
-      <c r="AG41" s="20"/>
-      <c r="AH41" s="20"/>
-      <c r="AI41" s="20"/>
-      <c r="AJ41" s="20"/>
-      <c r="AK41" s="20"/>
-      <c r="AL41" s="20"/>
-      <c r="AM41" s="20"/>
-      <c r="AN41" s="20"/>
-      <c r="AO41" s="20"/>
-      <c r="AP41" s="20"/>
-      <c r="AQ41" s="20"/>
-      <c r="AR41" s="20"/>
-      <c r="AS41" s="21"/>
-      <c r="AT41" s="22"/>
-      <c r="AU41" s="22"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="8"/>
+      <c r="N41" s="24"/>
+      <c r="O41" s="24"/>
+      <c r="AS41" s="24"/>
+      <c r="AT41" s="24"/>
     </row>
     <row r="42" spans="1:47" x14ac:dyDescent="0.3">
       <c r="C42" s="8"/>
@@ -3510,8 +3460,6 @@
       <c r="D44" s="8"/>
       <c r="E44" s="8"/>
       <c r="F44" s="8"/>
-      <c r="N44" s="24"/>
-      <c r="O44" s="24"/>
       <c r="AS44" s="24"/>
       <c r="AT44" s="24"/>
     </row>
@@ -3520,8 +3468,6 @@
       <c r="D45" s="8"/>
       <c r="E45" s="8"/>
       <c r="F45" s="8"/>
-      <c r="AS45" s="24"/>
-      <c r="AT45" s="24"/>
     </row>
     <row r="46" spans="1:47" x14ac:dyDescent="0.3">
       <c r="C46" s="8"/>
@@ -3534,12 +3480,6 @@
       <c r="D47" s="8"/>
       <c r="E47" s="8"/>
       <c r="F47" s="8"/>
-    </row>
-    <row r="48" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="C48" s="8"/>
-      <c r="D48" s="8"/>
-      <c r="E48" s="8"/>
-      <c r="F48" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -3553,37 +3493,37 @@
     <mergeCell ref="E4:F4"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A40:AP40 B6:B34">
+  <conditionalFormatting sqref="A39:AP39 B6:B33">
     <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>"Complete"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AT40:AU40">
+  <conditionalFormatting sqref="AT39:AU39">
     <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>"Complete"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B36">
+  <conditionalFormatting sqref="B35">
     <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"Complete"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B37">
+  <conditionalFormatting sqref="B36">
     <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"Complete"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B39">
+  <conditionalFormatting sqref="B38">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"Complete"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B38">
+  <conditionalFormatting sqref="B37">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Complete"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B35">
+  <conditionalFormatting sqref="B34">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Complete"</formula>
     </cfRule>

</xml_diff>